<commit_message>
improve scan flow and fix icon loading
</commit_message>
<xml_diff>
--- a/ex/TestOrder.xlsx
+++ b/ex/TestOrder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Project\ex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5170C76E-5514-4F3F-9393-CB09872BEC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EA80AE-80E5-40B6-B91B-27696E5993C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B28C14C4-DB55-46DE-808C-9598A1A4B3F2}"/>
   </bookViews>
@@ -449,7 +449,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,12 +465,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -511,7 +505,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,7 +897,7 @@
   <dimension ref="B1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +971,7 @@
       <c r="E2" s="3">
         <v>46051</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1019,7 +1012,7 @@
       <c r="E3" s="3">
         <v>46051</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1060,7 +1053,7 @@
       <c r="E4" s="3">
         <v>46051</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1101,7 +1094,7 @@
       <c r="E5" s="3">
         <v>46051</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>23</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -1142,7 +1135,7 @@
       <c r="E6" s="3">
         <v>46051</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -1183,7 +1176,7 @@
       <c r="E7" s="3">
         <v>46051</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1224,7 +1217,7 @@
       <c r="E8" s="3">
         <v>46051</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>67</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1265,7 +1258,7 @@
       <c r="E9" s="3">
         <v>46051</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1306,7 +1299,7 @@
       <c r="E10" s="3">
         <v>46051</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>6</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -1347,7 +1340,7 @@
       <c r="E11" s="3">
         <v>46051</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>44</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1388,7 +1381,7 @@
       <c r="E12" s="3">
         <v>46051</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -1429,7 +1422,7 @@
       <c r="E13" s="3">
         <v>46051</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -1470,7 +1463,7 @@
       <c r="E14" s="3">
         <v>46051</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>25</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1511,7 +1504,7 @@
       <c r="E15" s="3">
         <v>46051</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>18</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -1552,7 +1545,7 @@
       <c r="E16" s="3">
         <v>46051</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -1593,7 +1586,7 @@
       <c r="E17" s="3">
         <v>46051</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>1</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -1634,7 +1627,7 @@
       <c r="E18" s="3">
         <v>46051</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>99</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -1675,7 +1668,7 @@
       <c r="E19" s="3">
         <v>46051</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -1716,7 +1709,7 @@
       <c r="E20" s="3">
         <v>46051</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>19</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -1757,7 +1750,7 @@
       <c r="E21" s="3">
         <v>46051</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -1798,7 +1791,7 @@
       <c r="E22" s="3">
         <v>46051</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -1839,7 +1832,7 @@
       <c r="E23" s="3">
         <v>46051</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="5">
         <v>10</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -1880,7 +1873,7 @@
       <c r="E24" s="3">
         <v>46051</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <v>3</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -1921,7 +1914,7 @@
       <c r="E25" s="3">
         <v>46051</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <v>41</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -1962,7 +1955,7 @@
       <c r="E26" s="3">
         <v>46051</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <v>39</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -2003,7 +1996,7 @@
       <c r="E27" s="3">
         <v>46051</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <v>86</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -2044,7 +2037,7 @@
       <c r="E28" s="3">
         <v>46051</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <v>85</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -2085,7 +2078,7 @@
       <c r="E29" s="3">
         <v>46051</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="5">
         <v>20</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -2126,7 +2119,7 @@
       <c r="E30" s="3">
         <v>46051</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="5">
         <v>47</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -2182,15 +2175,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005257A1C43438D5419D3A082C8961659E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dbed44db3001106191f8497c6665d89b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="abae5456-feed-4704-ade7-be65738273c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e57d05feff9844251ace9b83539cc13f" ns3:_="">
     <xsd:import namespace="abae5456-feed-4704-ade7-be65738273c5"/>
@@ -2334,6 +2318,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{498E274B-AA7B-4099-B6DE-4DF00F51946B}">
   <ds:schemaRefs>
@@ -2351,14 +2344,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8566CFD2-36A0-41A0-8E51-6DC861FE055E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3471EC89-8C44-412E-930F-07F8A18DC078}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2374,4 +2359,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8566CFD2-36A0-41A0-8E51-6DC861FE055E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>